<commit_message>
Commit des docs du DDD
</commit_message>
<xml_diff>
--- a/Docs/ProjetAcsi_DDD.xlsx
+++ b/Docs/ProjetAcsi_DDD.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\quent_000\Desktop\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="60" windowWidth="20115" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="60" windowWidth="20112" windowHeight="8016"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -16,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="44">
   <si>
     <t>I/ Dictionnaire des données</t>
   </si>
@@ -39,99 +44,27 @@
     <t>Format/Observations</t>
   </si>
   <si>
-    <t>login</t>
-  </si>
-  <si>
-    <t>mdp</t>
-  </si>
-  <si>
-    <t>adr_mail</t>
-  </si>
-  <si>
-    <t>libelle_quiz</t>
-  </si>
-  <si>
-    <t>nbr_question</t>
-  </si>
-  <si>
     <t>difficulte_quiz</t>
   </si>
   <si>
-    <t>temps_quiz</t>
-  </si>
-  <si>
-    <t>statut</t>
-  </si>
-  <si>
     <t>id_quiz</t>
   </si>
   <si>
     <t>id_question</t>
   </si>
   <si>
-    <t>nbr_rep_total</t>
-  </si>
-  <si>
-    <t>nbr_rep_juste</t>
-  </si>
-  <si>
-    <t>quest_text</t>
-  </si>
-  <si>
-    <t>quest_img</t>
-  </si>
-  <si>
-    <t>rep_text</t>
-  </si>
-  <si>
-    <t>rep_img</t>
-  </si>
-  <si>
     <t>statut_rep</t>
   </si>
   <si>
     <t>score_usr_quiz</t>
   </si>
   <si>
-    <t>score_moyen_quiz</t>
-  </si>
-  <si>
-    <t>nbr_participant_quiz</t>
-  </si>
-  <si>
-    <t>temps_moy_usr_quiz</t>
-  </si>
-  <si>
-    <t>nbr_quiz_joue</t>
-  </si>
-  <si>
-    <t>nbr_quiz_cree_admin</t>
-  </si>
-  <si>
-    <t>nbr_quiz_total</t>
-  </si>
-  <si>
     <t>AN</t>
   </si>
   <si>
-    <t>L</t>
-  </si>
-  <si>
     <t>N</t>
   </si>
   <si>
-    <t>1=facile, 2=moyen etc.</t>
-  </si>
-  <si>
-    <t>DH</t>
-  </si>
-  <si>
-    <t>HH:MM:SS</t>
-  </si>
-  <si>
-    <t>&gt;= 2</t>
-  </si>
-  <si>
     <t>F</t>
   </si>
   <si>
@@ -142,6 +75,84 @@
   </si>
   <si>
     <t>C</t>
+  </si>
+  <si>
+    <t>login_usr</t>
+  </si>
+  <si>
+    <t>mdp_usr</t>
+  </si>
+  <si>
+    <t>adr_mail_usr</t>
+  </si>
+  <si>
+    <t>nb_quiz_joue</t>
+  </si>
+  <si>
+    <t>nb_partie_joue</t>
+  </si>
+  <si>
+    <t>login_admin</t>
+  </si>
+  <si>
+    <t>mdp_admin</t>
+  </si>
+  <si>
+    <t>adr_mail_admin</t>
+  </si>
+  <si>
+    <t>nb_quiz_cree</t>
+  </si>
+  <si>
+    <t>id_rep</t>
+  </si>
+  <si>
+    <t>text_rep</t>
+  </si>
+  <si>
+    <t>img_rep</t>
+  </si>
+  <si>
+    <t>nom_quiz</t>
+  </si>
+  <si>
+    <t>minute_quiz</t>
+  </si>
+  <si>
+    <t>seconde_quiz</t>
+  </si>
+  <si>
+    <t>heure_quiz</t>
+  </si>
+  <si>
+    <t>nb_question</t>
+  </si>
+  <si>
+    <t>categorie_quiz</t>
+  </si>
+  <si>
+    <t>nb_rep_total</t>
+  </si>
+  <si>
+    <t>nb_rep_juste</t>
+  </si>
+  <si>
+    <t>text_quest</t>
+  </si>
+  <si>
+    <t>img_quest</t>
+  </si>
+  <si>
+    <t>id_partie</t>
+  </si>
+  <si>
+    <t>heure_usr_quiz</t>
+  </si>
+  <si>
+    <t>minute_usr_quiz</t>
+  </si>
+  <si>
+    <t>seconde_usr_quiz</t>
   </si>
 </sst>
 </file>
@@ -177,8 +188,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -191,6 +205,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -239,7 +256,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -274,7 +291,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -483,26 +500,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F27"/>
+  <dimension ref="A1:F34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.42578125" style="1"/>
-    <col min="2" max="2" width="22.140625" customWidth="1"/>
-    <col min="3" max="3" width="9.42578125" customWidth="1"/>
-    <col min="6" max="6" width="20.85546875" customWidth="1"/>
+    <col min="1" max="1" width="11.44140625" style="1"/>
+    <col min="2" max="2" width="22.109375" customWidth="1"/>
+    <col min="3" max="3" width="9.44140625" customWidth="1"/>
+    <col min="6" max="6" width="20.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="2"/>
+    </row>
+    <row r="3" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -522,424 +540,537 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>31</v>
+        <v>12</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>40</v>
+        <v>16</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>8</v>
+        <v>19</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>31</v>
+        <v>12</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>40</v>
+        <v>16</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>3</v>
       </c>
       <c r="B6" t="s">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>31</v>
+        <v>12</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>40</v>
+        <v>16</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>4</v>
       </c>
       <c r="B7" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>32</v>
+        <v>13</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>40</v>
+        <v>17</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>5</v>
       </c>
       <c r="B8" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>33</v>
+        <v>13</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>41</v>
+        <v>17</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>6</v>
       </c>
       <c r="B9" t="s">
-        <v>10</v>
+        <v>23</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>31</v>
+        <v>12</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>40</v>
+        <v>16</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>7</v>
       </c>
       <c r="B10" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>33</v>
+        <v>12</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>41</v>
+        <v>16</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>8</v>
       </c>
       <c r="B11" t="s">
-        <v>12</v>
+        <v>25</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>33</v>
+        <v>12</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>40</v>
+        <v>16</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="F11" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>9</v>
       </c>
       <c r="B12" t="s">
-        <v>13</v>
+        <v>26</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>35</v>
+        <v>13</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>40</v>
+        <v>17</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="F12" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>10</v>
       </c>
       <c r="B13" t="s">
-        <v>16</v>
+        <v>27</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>33</v>
+        <v>13</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>41</v>
+        <v>17</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>11</v>
       </c>
       <c r="B14" t="s">
-        <v>17</v>
+        <v>28</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>33</v>
+        <v>12</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>40</v>
+        <v>16</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="F14" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <v>12</v>
       </c>
       <c r="B15" t="s">
-        <v>18</v>
+        <v>29</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>33</v>
+        <v>12</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>40</v>
+        <v>16</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <v>13</v>
       </c>
       <c r="B16" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>31</v>
+        <v>13</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>40</v>
+        <v>16</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <v>14</v>
       </c>
       <c r="B17" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>31</v>
+        <v>13</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>40</v>
+        <v>17</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <v>15</v>
       </c>
       <c r="B18" t="s">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>31</v>
+        <v>13</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>40</v>
+        <v>16</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <v>16</v>
       </c>
       <c r="B19" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>31</v>
+        <v>12</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>40</v>
+        <v>16</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <v>17</v>
       </c>
       <c r="B20" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>32</v>
+        <v>13</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>40</v>
+        <v>16</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <v>18</v>
       </c>
       <c r="B21" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>33</v>
+        <v>13</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>41</v>
+        <v>16</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
         <v>19</v>
       </c>
       <c r="B22" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>33</v>
+        <v>13</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>41</v>
+        <v>16</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
         <v>20</v>
       </c>
       <c r="B23" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>33</v>
+        <v>13</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>41</v>
+        <v>16</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
         <v>21</v>
       </c>
       <c r="B24" t="s">
-        <v>26</v>
+        <v>35</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>33</v>
+        <v>12</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>41</v>
+        <v>16</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
         <v>22</v>
       </c>
       <c r="B25" t="s">
-        <v>27</v>
+        <v>9</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>35</v>
+        <v>13</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>41</v>
+        <v>17</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" s="1">
         <v>23</v>
       </c>
       <c r="B26" t="s">
-        <v>28</v>
+        <v>36</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>33</v>
+        <v>13</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>41</v>
+        <v>16</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" s="1">
         <v>24</v>
       </c>
       <c r="B27" t="s">
+        <v>37</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A28" s="1">
+        <v>25</v>
+      </c>
+      <c r="B28" t="s">
+        <v>38</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A29" s="1">
+        <v>26</v>
+      </c>
+      <c r="B29" t="s">
+        <v>39</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A30" s="1">
+        <v>27</v>
+      </c>
+      <c r="B30" t="s">
+        <v>40</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A31" s="1">
+        <v>28</v>
+      </c>
+      <c r="B31" t="s">
+        <v>11</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A32" s="1">
+        <v>29</v>
+      </c>
+      <c r="B32" t="s">
+        <v>41</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A33" s="1">
         <v>30</v>
       </c>
-      <c r="C27" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D27" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="E27" s="1" t="s">
-        <v>39</v>
+      <c r="B33" t="s">
+        <v>42</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A34" s="1">
+        <v>31</v>
+      </c>
+      <c r="B34" t="s">
+        <v>43</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:B1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -950,7 +1081,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -962,7 +1093,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>